<commit_message>
Adjust user reports according to their tasks
</commit_message>
<xml_diff>
--- a/public/templates/report_templateV5.xlsx
+++ b/public/templates/report_templateV5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j1m-1\OneDrive\Documentos\jim\Quisvar\quisvar_proyect_ft\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gpro1\MyFiles\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356018BC-B95E-4E5A-94BC-1C1E12A84C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B3DCBE-16B8-4990-BCE8-B6C091279412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="_Hlk78726999" localSheetId="1">REPORTE!#REF!</definedName>
     <definedName name="_Hlk87049115" localSheetId="1">REPORTE!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">LIQUIDACION!$A$1:$BD$173</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">REPORTE!$A$1:$K$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">REPORTE!$A$1:$K$36</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">LIQUIDACION!$1:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">REPORTE!$1:$26</definedName>
   </definedNames>
@@ -32,6 +32,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1671,13 +1682,13 @@
     <t>(%) Avanzado</t>
   </si>
   <si>
-    <t>(%) Adelanto</t>
-  </si>
-  <si>
     <t>PERIODO DE TRABAJO(Dias)</t>
   </si>
   <si>
     <t>TOTAL DE DESCUENTO LICENCIA:</t>
+  </si>
+  <si>
+    <t>Dias Meta</t>
   </si>
 </sst>
 </file>
@@ -1685,13 +1696,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="44" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="00.00.00.00"/>
-    <numFmt numFmtId="165" formatCode="00.00.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;S/&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="&quot;S/&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="00.00.00.00"/>
+    <numFmt numFmtId="166" formatCode="00.00.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;S/&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="&quot;S/&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="43" x14ac:knownFonts="1">
     <font>
@@ -3070,9 +3081,9 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -3111,10 +3122,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3382,19 +3393,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3403,13 +3420,7 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3489,7 +3500,7 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3507,7 +3518,7 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3522,13 +3533,13 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="9" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="9" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3549,7 +3560,7 @@
     <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="27" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="27" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3558,7 +3569,7 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="24" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3576,7 +3587,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3633,7 +3644,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3654,7 +3665,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="31" fillId="9" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3675,10 +3686,10 @@
     <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="33" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="33" fillId="9" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3690,13 +3701,13 @@
     <xf numFmtId="0" fontId="21" fillId="9" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="40" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="40" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="41" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="41" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="42" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3714,6 +3725,108 @@
     <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -3732,107 +3845,56 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3843,16 +3905,55 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="35" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="35" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="35" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="35" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3867,106 +3968,16 @@
     <xf numFmtId="0" fontId="26" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="39" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="39" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="39" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="39" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="26" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="26" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4387,174 +4398,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="256" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="274"/>
-      <c r="C1" s="274"/>
-      <c r="D1" s="274"/>
-      <c r="E1" s="274"/>
-      <c r="F1" s="274"/>
-      <c r="G1" s="274"/>
-      <c r="H1" s="274"/>
-      <c r="I1" s="274"/>
-      <c r="J1" s="274"/>
-      <c r="K1" s="274"/>
-      <c r="L1" s="274"/>
-      <c r="M1" s="274"/>
-      <c r="N1" s="274"/>
-      <c r="O1" s="273" t="s">
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="255"/>
+      <c r="K1" s="255"/>
+      <c r="L1" s="255"/>
+      <c r="M1" s="255"/>
+      <c r="N1" s="255"/>
+      <c r="O1" s="254" t="s">
         <v>326</v>
       </c>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="273"/>
-      <c r="R1" s="273"/>
-      <c r="S1" s="273"/>
-      <c r="T1" s="273"/>
-      <c r="U1" s="273"/>
-      <c r="V1" s="273"/>
-      <c r="W1" s="273"/>
-      <c r="X1" s="273"/>
-      <c r="Y1" s="273"/>
-      <c r="Z1" s="273"/>
-      <c r="AA1" s="273"/>
-      <c r="AB1" s="273"/>
-      <c r="AC1" s="273"/>
-      <c r="AD1" s="273"/>
-      <c r="AE1" s="273"/>
-      <c r="AF1" s="273"/>
-      <c r="AG1" s="273"/>
-      <c r="AH1" s="274" t="s">
+      <c r="P1" s="254"/>
+      <c r="Q1" s="254"/>
+      <c r="R1" s="254"/>
+      <c r="S1" s="254"/>
+      <c r="T1" s="254"/>
+      <c r="U1" s="254"/>
+      <c r="V1" s="254"/>
+      <c r="W1" s="254"/>
+      <c r="X1" s="254"/>
+      <c r="Y1" s="254"/>
+      <c r="Z1" s="254"/>
+      <c r="AA1" s="254"/>
+      <c r="AB1" s="254"/>
+      <c r="AC1" s="254"/>
+      <c r="AD1" s="254"/>
+      <c r="AE1" s="254"/>
+      <c r="AF1" s="254"/>
+      <c r="AG1" s="254"/>
+      <c r="AH1" s="255" t="s">
         <v>320</v>
       </c>
-      <c r="AI1" s="274"/>
-      <c r="AJ1" s="274"/>
-      <c r="AK1" s="274"/>
-      <c r="AL1" s="271" t="s">
+      <c r="AI1" s="255"/>
+      <c r="AJ1" s="255"/>
+      <c r="AK1" s="255"/>
+      <c r="AL1" s="252" t="s">
         <v>327</v>
       </c>
-      <c r="AM1" s="271"/>
-      <c r="AN1" s="271"/>
-      <c r="AO1" s="271"/>
-      <c r="AP1" s="271"/>
-      <c r="AQ1" s="271"/>
-      <c r="AR1" s="271"/>
-      <c r="AS1" s="271"/>
-      <c r="AT1" s="271"/>
-      <c r="AU1" s="271"/>
-      <c r="AV1" s="271"/>
-      <c r="AW1" s="271"/>
-      <c r="AX1" s="271"/>
-      <c r="AY1" s="271"/>
-      <c r="AZ1" s="271"/>
-      <c r="BA1" s="271"/>
-      <c r="BB1" s="271"/>
-      <c r="BC1" s="271"/>
-      <c r="BD1" s="272"/>
+      <c r="AM1" s="252"/>
+      <c r="AN1" s="252"/>
+      <c r="AO1" s="252"/>
+      <c r="AP1" s="252"/>
+      <c r="AQ1" s="252"/>
+      <c r="AR1" s="252"/>
+      <c r="AS1" s="252"/>
+      <c r="AT1" s="252"/>
+      <c r="AU1" s="252"/>
+      <c r="AV1" s="252"/>
+      <c r="AW1" s="252"/>
+      <c r="AX1" s="252"/>
+      <c r="AY1" s="252"/>
+      <c r="AZ1" s="252"/>
+      <c r="BA1" s="252"/>
+      <c r="BB1" s="252"/>
+      <c r="BC1" s="252"/>
+      <c r="BD1" s="253"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="241" t="s">
+      <c r="A2" s="275" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="242"/>
+      <c r="B2" s="276"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="245" t="s">
+      <c r="D2" s="279" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="245"/>
-      <c r="F2" s="277" t="s">
+      <c r="E2" s="279"/>
+      <c r="F2" s="244" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="277"/>
-      <c r="H2" s="277"/>
-      <c r="I2" s="277"/>
-      <c r="J2" s="277"/>
-      <c r="K2" s="277"/>
-      <c r="L2" s="277"/>
-      <c r="M2" s="277"/>
-      <c r="N2" s="277"/>
-      <c r="O2" s="277"/>
-      <c r="P2" s="277"/>
-      <c r="Q2" s="277"/>
-      <c r="R2" s="277"/>
-      <c r="S2" s="277"/>
-      <c r="T2" s="277"/>
-      <c r="U2" s="277"/>
-      <c r="V2" s="277"/>
-      <c r="W2" s="277"/>
-      <c r="X2" s="277"/>
-      <c r="Y2" s="277"/>
-      <c r="Z2" s="277"/>
-      <c r="AA2" s="277"/>
-      <c r="AB2" s="277"/>
-      <c r="AC2" s="277"/>
-      <c r="AD2" s="277"/>
-      <c r="AE2" s="277"/>
-      <c r="AF2" s="277"/>
-      <c r="AG2" s="277"/>
-      <c r="AH2" s="277"/>
-      <c r="AI2" s="277"/>
-      <c r="AJ2" s="277"/>
-      <c r="AK2" s="277"/>
-      <c r="AL2" s="277"/>
-      <c r="AM2" s="277"/>
-      <c r="AN2" s="277"/>
-      <c r="AO2" s="277"/>
-      <c r="AP2" s="277"/>
-      <c r="AQ2" s="277"/>
-      <c r="AR2" s="277"/>
-      <c r="AS2" s="277"/>
-      <c r="AT2" s="277"/>
-      <c r="AU2" s="277"/>
-      <c r="AV2" s="277"/>
-      <c r="AW2" s="277"/>
-      <c r="AX2" s="277"/>
-      <c r="AY2" s="277"/>
-      <c r="AZ2" s="277"/>
-      <c r="BA2" s="277"/>
-      <c r="BB2" s="277"/>
-      <c r="BC2" s="277"/>
-      <c r="BD2" s="278"/>
+      <c r="G2" s="244"/>
+      <c r="H2" s="244"/>
+      <c r="I2" s="244"/>
+      <c r="J2" s="244"/>
+      <c r="K2" s="244"/>
+      <c r="L2" s="244"/>
+      <c r="M2" s="244"/>
+      <c r="N2" s="244"/>
+      <c r="O2" s="244"/>
+      <c r="P2" s="244"/>
+      <c r="Q2" s="244"/>
+      <c r="R2" s="244"/>
+      <c r="S2" s="244"/>
+      <c r="T2" s="244"/>
+      <c r="U2" s="244"/>
+      <c r="V2" s="244"/>
+      <c r="W2" s="244"/>
+      <c r="X2" s="244"/>
+      <c r="Y2" s="244"/>
+      <c r="Z2" s="244"/>
+      <c r="AA2" s="244"/>
+      <c r="AB2" s="244"/>
+      <c r="AC2" s="244"/>
+      <c r="AD2" s="244"/>
+      <c r="AE2" s="244"/>
+      <c r="AF2" s="244"/>
+      <c r="AG2" s="244"/>
+      <c r="AH2" s="244"/>
+      <c r="AI2" s="244"/>
+      <c r="AJ2" s="244"/>
+      <c r="AK2" s="244"/>
+      <c r="AL2" s="244"/>
+      <c r="AM2" s="244"/>
+      <c r="AN2" s="244"/>
+      <c r="AO2" s="244"/>
+      <c r="AP2" s="244"/>
+      <c r="AQ2" s="244"/>
+      <c r="AR2" s="244"/>
+      <c r="AS2" s="244"/>
+      <c r="AT2" s="244"/>
+      <c r="AU2" s="244"/>
+      <c r="AV2" s="244"/>
+      <c r="AW2" s="244"/>
+      <c r="AX2" s="244"/>
+      <c r="AY2" s="244"/>
+      <c r="AZ2" s="244"/>
+      <c r="BA2" s="244"/>
+      <c r="BB2" s="244"/>
+      <c r="BC2" s="244"/>
+      <c r="BD2" s="245"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="275" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="242"/>
+      <c r="B3" s="276"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="270" t="s">
+      <c r="D3" s="258" t="s">
         <v>331</v>
       </c>
-      <c r="E3" s="270"/>
+      <c r="E3" s="258"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="270" t="s">
+      <c r="I3" s="258" t="s">
         <v>335</v>
       </c>
-      <c r="J3" s="270"/>
-      <c r="K3" s="270"/>
-      <c r="L3" s="270"/>
-      <c r="M3" s="270"/>
-      <c r="N3" s="270"/>
-      <c r="O3" s="270"/>
-      <c r="P3" s="270"/>
-      <c r="Q3" s="270"/>
-      <c r="R3" s="280" t="s">
+      <c r="J3" s="258"/>
+      <c r="K3" s="258"/>
+      <c r="L3" s="258"/>
+      <c r="M3" s="258"/>
+      <c r="N3" s="258"/>
+      <c r="O3" s="258"/>
+      <c r="P3" s="258"/>
+      <c r="Q3" s="258"/>
+      <c r="R3" s="247" t="s">
         <v>337</v>
       </c>
-      <c r="S3" s="280"/>
-      <c r="T3" s="280"/>
-      <c r="U3" s="280"/>
-      <c r="V3" s="280"/>
-      <c r="W3" s="280"/>
-      <c r="X3" s="280"/>
+      <c r="S3" s="247"/>
+      <c r="T3" s="247"/>
+      <c r="U3" s="247"/>
+      <c r="V3" s="247"/>
+      <c r="W3" s="247"/>
+      <c r="X3" s="247"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4589,42 +4600,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="275" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="242"/>
+      <c r="B4" s="276"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="270" t="s">
+      <c r="D4" s="258" t="s">
         <v>332</v>
       </c>
-      <c r="E4" s="270"/>
+      <c r="E4" s="258"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="270" t="s">
+      <c r="I4" s="258" t="s">
         <v>336</v>
       </c>
-      <c r="J4" s="270"/>
-      <c r="K4" s="270"/>
-      <c r="L4" s="270"/>
-      <c r="M4" s="270"/>
-      <c r="N4" s="270"/>
-      <c r="O4" s="270"/>
-      <c r="P4" s="270"/>
-      <c r="Q4" s="270"/>
-      <c r="R4" s="280" t="s">
+      <c r="J4" s="258"/>
+      <c r="K4" s="258"/>
+      <c r="L4" s="258"/>
+      <c r="M4" s="258"/>
+      <c r="N4" s="258"/>
+      <c r="O4" s="258"/>
+      <c r="P4" s="258"/>
+      <c r="Q4" s="258"/>
+      <c r="R4" s="247" t="s">
         <v>338</v>
       </c>
-      <c r="S4" s="280"/>
-      <c r="T4" s="280"/>
-      <c r="U4" s="280"/>
-      <c r="V4" s="280"/>
-      <c r="W4" s="280"/>
-      <c r="X4" s="280"/>
+      <c r="S4" s="247"/>
+      <c r="T4" s="247"/>
+      <c r="U4" s="247"/>
+      <c r="V4" s="247"/>
+      <c r="W4" s="247"/>
+      <c r="X4" s="247"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4659,35 +4670,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="243" t="s">
+      <c r="A5" s="277" t="s">
         <v>302</v>
       </c>
-      <c r="B5" s="244"/>
+      <c r="B5" s="278"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="246" t="s">
+      <c r="D5" s="280" t="s">
         <v>333</v>
       </c>
-      <c r="E5" s="246"/>
-      <c r="F5" s="279" t="s">
+      <c r="E5" s="280"/>
+      <c r="F5" s="246" t="s">
         <v>334</v>
       </c>
-      <c r="G5" s="279"/>
-      <c r="H5" s="279"/>
-      <c r="I5" s="279"/>
-      <c r="J5" s="279"/>
-      <c r="K5" s="279"/>
-      <c r="L5" s="279"/>
-      <c r="M5" s="279"/>
-      <c r="N5" s="279"/>
-      <c r="O5" s="279"/>
-      <c r="P5" s="279"/>
-      <c r="Q5" s="279"/>
-      <c r="R5" s="279"/>
-      <c r="S5" s="279"/>
-      <c r="T5" s="279"/>
-      <c r="U5" s="279"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="246"/>
+      <c r="J5" s="246"/>
+      <c r="K5" s="246"/>
+      <c r="L5" s="246"/>
+      <c r="M5" s="246"/>
+      <c r="N5" s="246"/>
+      <c r="O5" s="246"/>
+      <c r="P5" s="246"/>
+      <c r="Q5" s="246"/>
+      <c r="R5" s="246"/>
+      <c r="S5" s="246"/>
+      <c r="T5" s="246"/>
+      <c r="U5" s="246"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4725,101 +4736,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="250" t="s">
+      <c r="A6" s="267" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="252" t="s">
+      <c r="B6" s="269" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="252" t="s">
+      <c r="C6" s="269" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="252" t="s">
+      <c r="D6" s="269" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="259" t="s">
+      <c r="E6" s="273" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="260"/>
-      <c r="G6" s="257" t="s">
+      <c r="F6" s="274"/>
+      <c r="G6" s="271" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="247" t="s">
+      <c r="H6" s="249" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="248"/>
-      <c r="J6" s="248"/>
-      <c r="K6" s="248"/>
-      <c r="L6" s="248"/>
-      <c r="M6" s="248"/>
-      <c r="N6" s="249"/>
-      <c r="O6" s="247" t="s">
+      <c r="I6" s="250"/>
+      <c r="J6" s="250"/>
+      <c r="K6" s="250"/>
+      <c r="L6" s="250"/>
+      <c r="M6" s="250"/>
+      <c r="N6" s="251"/>
+      <c r="O6" s="249" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="248"/>
-      <c r="Q6" s="248"/>
-      <c r="R6" s="248"/>
-      <c r="S6" s="248"/>
-      <c r="T6" s="248"/>
-      <c r="U6" s="249"/>
-      <c r="V6" s="247" t="s">
+      <c r="P6" s="250"/>
+      <c r="Q6" s="250"/>
+      <c r="R6" s="250"/>
+      <c r="S6" s="250"/>
+      <c r="T6" s="250"/>
+      <c r="U6" s="251"/>
+      <c r="V6" s="249" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="248"/>
-      <c r="X6" s="248"/>
-      <c r="Y6" s="248"/>
-      <c r="Z6" s="248"/>
-      <c r="AA6" s="248"/>
-      <c r="AB6" s="249"/>
-      <c r="AC6" s="247" t="s">
+      <c r="W6" s="250"/>
+      <c r="X6" s="250"/>
+      <c r="Y6" s="250"/>
+      <c r="Z6" s="250"/>
+      <c r="AA6" s="250"/>
+      <c r="AB6" s="251"/>
+      <c r="AC6" s="249" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="248"/>
-      <c r="AE6" s="248"/>
-      <c r="AF6" s="248"/>
-      <c r="AG6" s="248"/>
-      <c r="AH6" s="248"/>
-      <c r="AI6" s="249"/>
-      <c r="AJ6" s="247" t="s">
+      <c r="AD6" s="250"/>
+      <c r="AE6" s="250"/>
+      <c r="AF6" s="250"/>
+      <c r="AG6" s="250"/>
+      <c r="AH6" s="250"/>
+      <c r="AI6" s="251"/>
+      <c r="AJ6" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="248"/>
-      <c r="AL6" s="248"/>
-      <c r="AM6" s="248"/>
-      <c r="AN6" s="248"/>
-      <c r="AO6" s="248"/>
-      <c r="AP6" s="249"/>
-      <c r="AQ6" s="247" t="s">
+      <c r="AK6" s="250"/>
+      <c r="AL6" s="250"/>
+      <c r="AM6" s="250"/>
+      <c r="AN6" s="250"/>
+      <c r="AO6" s="250"/>
+      <c r="AP6" s="251"/>
+      <c r="AQ6" s="249" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="248"/>
-      <c r="AS6" s="248"/>
-      <c r="AT6" s="248"/>
-      <c r="AU6" s="248"/>
-      <c r="AV6" s="248"/>
-      <c r="AW6" s="249"/>
-      <c r="AX6" s="247" t="s">
+      <c r="AR6" s="250"/>
+      <c r="AS6" s="250"/>
+      <c r="AT6" s="250"/>
+      <c r="AU6" s="250"/>
+      <c r="AV6" s="250"/>
+      <c r="AW6" s="251"/>
+      <c r="AX6" s="249" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="248"/>
-      <c r="AZ6" s="248"/>
-      <c r="BA6" s="248"/>
-      <c r="BB6" s="248"/>
-      <c r="BC6" s="248"/>
-      <c r="BD6" s="249"/>
+      <c r="AY6" s="250"/>
+      <c r="AZ6" s="250"/>
+      <c r="BA6" s="250"/>
+      <c r="BB6" s="250"/>
+      <c r="BC6" s="250"/>
+      <c r="BD6" s="251"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="251"/>
-      <c r="B7" s="253"/>
-      <c r="C7" s="253"/>
-      <c r="D7" s="253"/>
+      <c r="A7" s="268"/>
+      <c r="B7" s="270"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>312</v>
       </c>
-      <c r="G7" s="258"/>
+      <c r="G7" s="272"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5093,7 +5104,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="254" t="s">
+      <c r="A10" s="263" t="s">
         <v>314</v>
       </c>
       <c r="B10" s="135"/>
@@ -5161,7 +5172,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="255"/>
+      <c r="A11" s="264"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5227,7 +5238,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="256"/>
+      <c r="A12" s="266"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5417,7 +5428,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="254" t="s">
+      <c r="A15" s="263" t="s">
         <v>315</v>
       </c>
       <c r="B15" s="135"/>
@@ -5487,7 +5498,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="255"/>
+      <c r="A16" s="264"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5555,7 +5566,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="255"/>
+      <c r="A17" s="264"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5623,7 +5634,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="255"/>
+      <c r="A18" s="264"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5691,7 +5702,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="255"/>
+      <c r="A19" s="264"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5759,7 +5770,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="255"/>
+      <c r="A20" s="264"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5827,7 +5838,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="255"/>
+      <c r="A21" s="264"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5895,7 +5906,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="255"/>
+      <c r="A22" s="264"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -5963,7 +5974,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="255"/>
+      <c r="A23" s="264"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -6031,7 +6042,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="255"/>
+      <c r="A24" s="264"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6099,7 +6110,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="255"/>
+      <c r="A25" s="264"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6167,7 +6178,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="255"/>
+      <c r="A26" s="264"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6235,7 +6246,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="255"/>
+      <c r="A27" s="264"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6303,7 +6314,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="255"/>
+      <c r="A28" s="264"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6371,7 +6382,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="255"/>
+      <c r="A29" s="264"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6439,7 +6450,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="256"/>
+      <c r="A30" s="266"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6569,7 +6580,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="254" t="s">
+      <c r="A32" s="263" t="s">
         <v>316</v>
       </c>
       <c r="B32" s="135"/>
@@ -6637,7 +6648,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="255"/>
+      <c r="A33" s="264"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6703,7 +6714,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="255"/>
+      <c r="A34" s="264"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6769,7 +6780,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="256"/>
+      <c r="A35" s="266"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6897,7 +6908,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="254" t="s">
+      <c r="A37" s="263" t="s">
         <v>317</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -6961,7 +6972,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="255"/>
+      <c r="A38" s="264"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -7029,7 +7040,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="255"/>
+      <c r="A39" s="264"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7097,7 +7108,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="255"/>
+      <c r="A40" s="264"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7159,7 +7170,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="255"/>
+      <c r="A41" s="264"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7227,7 +7238,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="255"/>
+      <c r="A42" s="264"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7289,7 +7300,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="255"/>
+      <c r="A43" s="264"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7353,7 +7364,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="255"/>
+      <c r="A44" s="264"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7419,7 +7430,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="255"/>
+      <c r="A45" s="264"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7485,7 +7496,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="255"/>
+      <c r="A46" s="264"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7547,7 +7558,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="255"/>
+      <c r="A47" s="264"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7615,7 +7626,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="255"/>
+      <c r="A48" s="264"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7683,7 +7694,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="255"/>
+      <c r="A49" s="264"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7751,7 +7762,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="255"/>
+      <c r="A50" s="264"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7819,7 +7830,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="255"/>
+      <c r="A51" s="264"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7881,7 +7892,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="255"/>
+      <c r="A52" s="264"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -7949,7 +7960,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="255"/>
+      <c r="A53" s="264"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -8017,7 +8028,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="255"/>
+      <c r="A54" s="264"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8079,7 +8090,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="255"/>
+      <c r="A55" s="264"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8145,7 +8156,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="255"/>
+      <c r="A56" s="264"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8213,7 +8224,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="255"/>
+      <c r="A57" s="264"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8281,7 +8292,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="255"/>
+      <c r="A58" s="264"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8347,7 +8358,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="255"/>
+      <c r="A59" s="264"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8415,7 +8426,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="255"/>
+      <c r="A60" s="264"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8483,7 +8494,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="255"/>
+      <c r="A61" s="264"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8545,7 +8556,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="255"/>
+      <c r="A62" s="264"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8613,7 +8624,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="255"/>
+      <c r="A63" s="264"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8681,7 +8692,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="255"/>
+      <c r="A64" s="264"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8743,7 +8754,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="255"/>
+      <c r="A65" s="264"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8811,7 +8822,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="255"/>
+      <c r="A66" s="264"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8873,7 +8884,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="255"/>
+      <c r="A67" s="264"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -8941,7 +8952,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="255"/>
+      <c r="A68" s="264"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -9003,7 +9014,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="255"/>
+      <c r="A69" s="264"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -9071,7 +9082,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="255"/>
+      <c r="A70" s="264"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9139,7 +9150,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="255"/>
+      <c r="A71" s="264"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9201,7 +9212,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="255"/>
+      <c r="A72" s="264"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9269,7 +9280,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="255"/>
+      <c r="A73" s="264"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9331,7 +9342,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="256"/>
+      <c r="A74" s="266"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9523,7 +9534,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="254" t="s">
+      <c r="A77" s="263" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9591,7 +9602,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="256"/>
+      <c r="A78" s="266"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9719,7 +9730,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="254" t="s">
+      <c r="A80" s="263" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9787,7 +9798,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="256"/>
+      <c r="A81" s="266"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9915,7 +9926,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="254" t="s">
+      <c r="A83" s="263" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -9983,7 +9994,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="256"/>
+      <c r="A84" s="266"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10173,7 +10184,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="254" t="s">
+      <c r="A87" s="263" t="s">
         <v>319</v>
       </c>
       <c r="B87" s="135"/>
@@ -10241,7 +10252,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="255"/>
+      <c r="A88" s="264"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10307,7 +10318,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="255"/>
+      <c r="A89" s="264"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10373,7 +10384,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="255"/>
+      <c r="A90" s="264"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10439,7 +10450,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="255"/>
+      <c r="A91" s="264"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10505,7 +10516,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="255"/>
+      <c r="A92" s="264"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10571,7 +10582,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="255"/>
+      <c r="A93" s="264"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10637,7 +10648,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="255"/>
+      <c r="A94" s="264"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10703,7 +10714,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="255"/>
+      <c r="A95" s="264"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10769,7 +10780,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="255"/>
+      <c r="A96" s="264"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10835,7 +10846,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="255"/>
+      <c r="A97" s="264"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10901,7 +10912,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="255"/>
+      <c r="A98" s="264"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -10967,7 +10978,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="255"/>
+      <c r="A99" s="264"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -11033,7 +11044,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="255"/>
+      <c r="A100" s="264"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11099,7 +11110,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="255"/>
+      <c r="A101" s="264"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11165,7 +11176,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="256"/>
+      <c r="A102" s="266"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11293,7 +11304,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="254" t="s">
+      <c r="A104" s="263" t="s">
         <v>318</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11357,7 +11368,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="255"/>
+      <c r="A105" s="264"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11425,7 +11436,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="255"/>
+      <c r="A106" s="264"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11487,7 +11498,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="255"/>
+      <c r="A107" s="264"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11555,7 +11566,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="255"/>
+      <c r="A108" s="264"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11623,7 +11634,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="255"/>
+      <c r="A109" s="264"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11685,7 +11696,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="255"/>
+      <c r="A110" s="264"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11753,7 +11764,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="255"/>
+      <c r="A111" s="264"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11815,7 +11826,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="255"/>
+      <c r="A112" s="264"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11883,7 +11894,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="255"/>
+      <c r="A113" s="264"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -11949,7 +11960,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="255"/>
+      <c r="A114" s="264"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -12015,7 +12026,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="255"/>
+      <c r="A115" s="264"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12077,7 +12088,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="255"/>
+      <c r="A116" s="264"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12145,7 +12156,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="255"/>
+      <c r="A117" s="264"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12213,7 +12224,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="255"/>
+      <c r="A118" s="264"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12281,7 +12292,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="255"/>
+      <c r="A119" s="264"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12349,7 +12360,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="255"/>
+      <c r="A120" s="264"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12411,7 +12422,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="255"/>
+      <c r="A121" s="264"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12479,7 +12490,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="255"/>
+      <c r="A122" s="264"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12547,7 +12558,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="255"/>
+      <c r="A123" s="264"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12609,7 +12620,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="255"/>
+      <c r="A124" s="264"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12673,7 +12684,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="255"/>
+      <c r="A125" s="264"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12739,7 +12750,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="255"/>
+      <c r="A126" s="264"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12805,7 +12816,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="255"/>
+      <c r="A127" s="264"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12869,7 +12880,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="255"/>
+      <c r="A128" s="264"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -12935,7 +12946,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="255"/>
+      <c r="A129" s="264"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -13001,7 +13012,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="255"/>
+      <c r="A130" s="264"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -13063,7 +13074,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="255"/>
+      <c r="A131" s="264"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13131,7 +13142,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="255"/>
+      <c r="A132" s="264"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13199,7 +13210,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="255"/>
+      <c r="A133" s="264"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13261,7 +13272,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="255"/>
+      <c r="A134" s="264"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13329,7 +13340,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="255"/>
+      <c r="A135" s="264"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13391,7 +13402,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="255"/>
+      <c r="A136" s="264"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13459,7 +13470,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="255"/>
+      <c r="A137" s="264"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13521,7 +13532,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="255"/>
+      <c r="A138" s="264"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13589,7 +13600,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="255"/>
+      <c r="A139" s="264"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13651,7 +13662,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="255"/>
+      <c r="A140" s="264"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13719,7 +13730,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="255"/>
+      <c r="A141" s="264"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13787,7 +13798,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="255"/>
+      <c r="A142" s="264"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13849,7 +13860,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="255"/>
+      <c r="A143" s="264"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13917,7 +13928,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="255"/>
+      <c r="A144" s="264"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -13979,7 +13990,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="255"/>
+      <c r="A145" s="264"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -14047,7 +14058,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="255"/>
+      <c r="A146" s="264"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14109,7 +14120,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="255"/>
+      <c r="A147" s="264"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14177,7 +14188,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="255"/>
+      <c r="A148" s="264"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14239,7 +14250,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="255"/>
+      <c r="A149" s="264"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14307,7 +14318,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="255"/>
+      <c r="A150" s="264"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14375,7 +14386,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="255"/>
+      <c r="A151" s="264"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14443,7 +14454,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="255"/>
+      <c r="A152" s="264"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14511,7 +14522,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="255"/>
+      <c r="A153" s="264"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14573,7 +14584,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="255"/>
+      <c r="A154" s="264"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14641,7 +14652,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="255"/>
+      <c r="A155" s="264"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14709,7 +14720,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="255"/>
+      <c r="A156" s="264"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14771,7 +14782,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="255"/>
+      <c r="A157" s="264"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14839,7 +14850,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="255"/>
+      <c r="A158" s="264"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14907,7 +14918,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="255"/>
+      <c r="A159" s="264"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -14975,7 +14986,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="255"/>
+      <c r="A160" s="264"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -15043,7 +15054,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="255"/>
+      <c r="A161" s="264"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15105,7 +15116,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="255"/>
+      <c r="A162" s="264"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15173,7 +15184,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="255"/>
+      <c r="A163" s="264"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15241,7 +15252,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="255"/>
+      <c r="A164" s="264"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15303,7 +15314,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="255"/>
+      <c r="A165" s="264"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15371,7 +15382,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="255"/>
+      <c r="A166" s="264"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15439,7 +15450,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="255"/>
+      <c r="A167" s="264"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15501,7 +15512,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="261"/>
+      <c r="A168" s="265"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15641,74 +15652,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="276" t="s">
+      <c r="E170" s="248" t="s">
         <v>324</v>
       </c>
-      <c r="F170" s="276"/>
-      <c r="G170" s="276"/>
-      <c r="H170" s="268"/>
-      <c r="I170" s="266"/>
-      <c r="J170" s="266"/>
-      <c r="K170" s="266">
+      <c r="F170" s="248"/>
+      <c r="G170" s="248"/>
+      <c r="H170" s="243"/>
+      <c r="I170" s="241"/>
+      <c r="J170" s="241"/>
+      <c r="K170" s="241">
         <v>500</v>
       </c>
-      <c r="L170" s="266"/>
-      <c r="M170" s="266"/>
-      <c r="N170" s="267"/>
-      <c r="O170" s="268"/>
-      <c r="P170" s="266"/>
-      <c r="Q170" s="266"/>
-      <c r="R170" s="266">
+      <c r="L170" s="241"/>
+      <c r="M170" s="241"/>
+      <c r="N170" s="242"/>
+      <c r="O170" s="243"/>
+      <c r="P170" s="241"/>
+      <c r="Q170" s="241"/>
+      <c r="R170" s="241">
         <v>500</v>
       </c>
-      <c r="S170" s="266"/>
-      <c r="T170" s="266"/>
-      <c r="U170" s="267"/>
-      <c r="V170" s="268"/>
-      <c r="W170" s="266"/>
-      <c r="X170" s="266"/>
-      <c r="Y170" s="266">
+      <c r="S170" s="241"/>
+      <c r="T170" s="241"/>
+      <c r="U170" s="242"/>
+      <c r="V170" s="243"/>
+      <c r="W170" s="241"/>
+      <c r="X170" s="241"/>
+      <c r="Y170" s="241">
         <v>500</v>
       </c>
-      <c r="Z170" s="266"/>
-      <c r="AA170" s="266"/>
-      <c r="AB170" s="267"/>
-      <c r="AC170" s="268"/>
-      <c r="AD170" s="266"/>
-      <c r="AE170" s="266"/>
-      <c r="AF170" s="266">
+      <c r="Z170" s="241"/>
+      <c r="AA170" s="241"/>
+      <c r="AB170" s="242"/>
+      <c r="AC170" s="243"/>
+      <c r="AD170" s="241"/>
+      <c r="AE170" s="241"/>
+      <c r="AF170" s="241">
         <v>500</v>
       </c>
-      <c r="AG170" s="266"/>
-      <c r="AH170" s="266"/>
-      <c r="AI170" s="267"/>
-      <c r="AJ170" s="268"/>
-      <c r="AK170" s="266"/>
-      <c r="AL170" s="266"/>
-      <c r="AM170" s="266">
+      <c r="AG170" s="241"/>
+      <c r="AH170" s="241"/>
+      <c r="AI170" s="242"/>
+      <c r="AJ170" s="243"/>
+      <c r="AK170" s="241"/>
+      <c r="AL170" s="241"/>
+      <c r="AM170" s="241">
         <v>500</v>
       </c>
-      <c r="AN170" s="266"/>
-      <c r="AO170" s="266"/>
-      <c r="AP170" s="267"/>
-      <c r="AQ170" s="268"/>
-      <c r="AR170" s="266"/>
-      <c r="AS170" s="266"/>
-      <c r="AT170" s="266">
+      <c r="AN170" s="241"/>
+      <c r="AO170" s="241"/>
+      <c r="AP170" s="242"/>
+      <c r="AQ170" s="243"/>
+      <c r="AR170" s="241"/>
+      <c r="AS170" s="241"/>
+      <c r="AT170" s="241">
         <v>500</v>
       </c>
-      <c r="AU170" s="266"/>
-      <c r="AV170" s="266"/>
-      <c r="AW170" s="267"/>
-      <c r="AX170" s="268"/>
-      <c r="AY170" s="266"/>
-      <c r="AZ170" s="266"/>
-      <c r="BA170" s="266">
+      <c r="AU170" s="241"/>
+      <c r="AV170" s="241"/>
+      <c r="AW170" s="242"/>
+      <c r="AX170" s="243"/>
+      <c r="AY170" s="241"/>
+      <c r="AZ170" s="241"/>
+      <c r="BA170" s="241">
         <v>500</v>
       </c>
-      <c r="BB170" s="266"/>
-      <c r="BC170" s="266"/>
-      <c r="BD170" s="267"/>
+      <c r="BB170" s="241"/>
+      <c r="BC170" s="241"/>
+      <c r="BD170" s="242"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15720,74 +15731,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="276" t="s">
+      <c r="E171" s="248" t="s">
         <v>323</v>
       </c>
-      <c r="F171" s="276"/>
-      <c r="G171" s="276"/>
-      <c r="H171" s="268"/>
-      <c r="I171" s="266"/>
-      <c r="J171" s="266"/>
-      <c r="K171" s="266">
+      <c r="F171" s="248"/>
+      <c r="G171" s="248"/>
+      <c r="H171" s="243"/>
+      <c r="I171" s="241"/>
+      <c r="J171" s="241"/>
+      <c r="K171" s="241">
         <v>630</v>
       </c>
-      <c r="L171" s="266"/>
-      <c r="M171" s="266"/>
-      <c r="N171" s="267"/>
-      <c r="O171" s="268"/>
-      <c r="P171" s="266"/>
-      <c r="Q171" s="266"/>
-      <c r="R171" s="266">
+      <c r="L171" s="241"/>
+      <c r="M171" s="241"/>
+      <c r="N171" s="242"/>
+      <c r="O171" s="243"/>
+      <c r="P171" s="241"/>
+      <c r="Q171" s="241"/>
+      <c r="R171" s="241">
         <v>630</v>
       </c>
-      <c r="S171" s="266"/>
-      <c r="T171" s="266"/>
-      <c r="U171" s="267"/>
-      <c r="V171" s="268"/>
-      <c r="W171" s="266"/>
-      <c r="X171" s="266"/>
-      <c r="Y171" s="266">
+      <c r="S171" s="241"/>
+      <c r="T171" s="241"/>
+      <c r="U171" s="242"/>
+      <c r="V171" s="243"/>
+      <c r="W171" s="241"/>
+      <c r="X171" s="241"/>
+      <c r="Y171" s="241">
         <v>630</v>
       </c>
-      <c r="Z171" s="266"/>
-      <c r="AA171" s="266"/>
-      <c r="AB171" s="267"/>
-      <c r="AC171" s="268"/>
-      <c r="AD171" s="266"/>
-      <c r="AE171" s="266"/>
-      <c r="AF171" s="266">
+      <c r="Z171" s="241"/>
+      <c r="AA171" s="241"/>
+      <c r="AB171" s="242"/>
+      <c r="AC171" s="243"/>
+      <c r="AD171" s="241"/>
+      <c r="AE171" s="241"/>
+      <c r="AF171" s="241">
         <v>630</v>
       </c>
-      <c r="AG171" s="266"/>
-      <c r="AH171" s="266"/>
-      <c r="AI171" s="267"/>
-      <c r="AJ171" s="268"/>
-      <c r="AK171" s="266"/>
-      <c r="AL171" s="266"/>
-      <c r="AM171" s="266">
+      <c r="AG171" s="241"/>
+      <c r="AH171" s="241"/>
+      <c r="AI171" s="242"/>
+      <c r="AJ171" s="243"/>
+      <c r="AK171" s="241"/>
+      <c r="AL171" s="241"/>
+      <c r="AM171" s="241">
         <v>630</v>
       </c>
-      <c r="AN171" s="266"/>
-      <c r="AO171" s="266"/>
-      <c r="AP171" s="267"/>
-      <c r="AQ171" s="268"/>
-      <c r="AR171" s="266"/>
-      <c r="AS171" s="266"/>
-      <c r="AT171" s="266">
+      <c r="AN171" s="241"/>
+      <c r="AO171" s="241"/>
+      <c r="AP171" s="242"/>
+      <c r="AQ171" s="243"/>
+      <c r="AR171" s="241"/>
+      <c r="AS171" s="241"/>
+      <c r="AT171" s="241">
         <v>630</v>
       </c>
-      <c r="AU171" s="266"/>
-      <c r="AV171" s="266"/>
-      <c r="AW171" s="267"/>
-      <c r="AX171" s="268"/>
-      <c r="AY171" s="266"/>
-      <c r="AZ171" s="266"/>
-      <c r="BA171" s="266">
+      <c r="AU171" s="241"/>
+      <c r="AV171" s="241"/>
+      <c r="AW171" s="242"/>
+      <c r="AX171" s="243"/>
+      <c r="AY171" s="241"/>
+      <c r="AZ171" s="241"/>
+      <c r="BA171" s="241">
         <v>630</v>
       </c>
-      <c r="BB171" s="266"/>
-      <c r="BC171" s="266"/>
-      <c r="BD171" s="267"/>
+      <c r="BB171" s="241"/>
+      <c r="BC171" s="241"/>
+      <c r="BD171" s="242"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15799,74 +15810,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="269" t="s">
+      <c r="E172" s="257" t="s">
         <v>307</v>
       </c>
-      <c r="F172" s="269"/>
-      <c r="G172" s="269"/>
-      <c r="H172" s="264"/>
-      <c r="I172" s="265"/>
-      <c r="J172" s="265"/>
-      <c r="K172" s="262">
+      <c r="F172" s="257"/>
+      <c r="G172" s="257"/>
+      <c r="H172" s="259"/>
+      <c r="I172" s="260"/>
+      <c r="J172" s="260"/>
+      <c r="K172" s="261">
         <v>44607</v>
       </c>
-      <c r="L172" s="262"/>
-      <c r="M172" s="262"/>
-      <c r="N172" s="263"/>
-      <c r="O172" s="264"/>
-      <c r="P172" s="265"/>
-      <c r="Q172" s="265"/>
-      <c r="R172" s="262">
+      <c r="L172" s="261"/>
+      <c r="M172" s="261"/>
+      <c r="N172" s="262"/>
+      <c r="O172" s="259"/>
+      <c r="P172" s="260"/>
+      <c r="Q172" s="260"/>
+      <c r="R172" s="261">
         <v>44607</v>
       </c>
-      <c r="S172" s="262"/>
-      <c r="T172" s="262"/>
-      <c r="U172" s="263"/>
-      <c r="V172" s="264"/>
-      <c r="W172" s="265"/>
-      <c r="X172" s="265"/>
-      <c r="Y172" s="262">
+      <c r="S172" s="261"/>
+      <c r="T172" s="261"/>
+      <c r="U172" s="262"/>
+      <c r="V172" s="259"/>
+      <c r="W172" s="260"/>
+      <c r="X172" s="260"/>
+      <c r="Y172" s="261">
         <v>44607</v>
       </c>
-      <c r="Z172" s="262"/>
-      <c r="AA172" s="262"/>
-      <c r="AB172" s="263"/>
-      <c r="AC172" s="264"/>
-      <c r="AD172" s="265"/>
-      <c r="AE172" s="265"/>
-      <c r="AF172" s="262">
+      <c r="Z172" s="261"/>
+      <c r="AA172" s="261"/>
+      <c r="AB172" s="262"/>
+      <c r="AC172" s="259"/>
+      <c r="AD172" s="260"/>
+      <c r="AE172" s="260"/>
+      <c r="AF172" s="261">
         <v>44607</v>
       </c>
-      <c r="AG172" s="262"/>
-      <c r="AH172" s="262"/>
-      <c r="AI172" s="263"/>
-      <c r="AJ172" s="264"/>
-      <c r="AK172" s="265"/>
-      <c r="AL172" s="265"/>
-      <c r="AM172" s="262">
+      <c r="AG172" s="261"/>
+      <c r="AH172" s="261"/>
+      <c r="AI172" s="262"/>
+      <c r="AJ172" s="259"/>
+      <c r="AK172" s="260"/>
+      <c r="AL172" s="260"/>
+      <c r="AM172" s="261">
         <v>44607</v>
       </c>
-      <c r="AN172" s="262"/>
-      <c r="AO172" s="262"/>
-      <c r="AP172" s="263"/>
-      <c r="AQ172" s="264"/>
-      <c r="AR172" s="265"/>
-      <c r="AS172" s="265"/>
-      <c r="AT172" s="262">
+      <c r="AN172" s="261"/>
+      <c r="AO172" s="261"/>
+      <c r="AP172" s="262"/>
+      <c r="AQ172" s="259"/>
+      <c r="AR172" s="260"/>
+      <c r="AS172" s="260"/>
+      <c r="AT172" s="261">
         <v>44607</v>
       </c>
-      <c r="AU172" s="262"/>
-      <c r="AV172" s="262"/>
-      <c r="AW172" s="263"/>
-      <c r="AX172" s="264"/>
-      <c r="AY172" s="265"/>
-      <c r="AZ172" s="265"/>
-      <c r="BA172" s="262">
+      <c r="AU172" s="261"/>
+      <c r="AV172" s="261"/>
+      <c r="AW172" s="262"/>
+      <c r="AX172" s="259"/>
+      <c r="AY172" s="260"/>
+      <c r="AZ172" s="260"/>
+      <c r="BA172" s="261">
         <v>44607</v>
       </c>
-      <c r="BB172" s="262"/>
-      <c r="BC172" s="262"/>
-      <c r="BD172" s="263"/>
+      <c r="BB172" s="261"/>
+      <c r="BC172" s="261"/>
+      <c r="BD172" s="262"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -15991,6 +16002,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="AJ6:AP6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="V6:AB6"/>
+    <mergeCell ref="AC6:AI6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A104:A168"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A87:A102"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A74"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="R172:U172"/>
+    <mergeCell ref="V172:X172"/>
+    <mergeCell ref="Y170:AB170"/>
+    <mergeCell ref="AC170:AE170"/>
+    <mergeCell ref="AF170:AI170"/>
+    <mergeCell ref="V170:X170"/>
+    <mergeCell ref="R170:U170"/>
+    <mergeCell ref="AQ172:AS172"/>
+    <mergeCell ref="AT172:AW172"/>
+    <mergeCell ref="AX172:AZ172"/>
+    <mergeCell ref="BA172:BD172"/>
+    <mergeCell ref="Y172:AB172"/>
+    <mergeCell ref="AC172:AE172"/>
+    <mergeCell ref="AF172:AI172"/>
+    <mergeCell ref="AJ172:AL172"/>
+    <mergeCell ref="AM172:AP172"/>
+    <mergeCell ref="E172:G172"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:Q3"/>
+    <mergeCell ref="I4:Q4"/>
+    <mergeCell ref="H172:J172"/>
+    <mergeCell ref="K172:N172"/>
+    <mergeCell ref="O172:Q172"/>
+    <mergeCell ref="H170:J170"/>
+    <mergeCell ref="K170:N170"/>
+    <mergeCell ref="O170:Q170"/>
+    <mergeCell ref="AL1:BD1"/>
+    <mergeCell ref="O1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="E171:G171"/>
+    <mergeCell ref="H171:J171"/>
+    <mergeCell ref="K171:N171"/>
+    <mergeCell ref="O171:Q171"/>
+    <mergeCell ref="R171:U171"/>
+    <mergeCell ref="V171:X171"/>
+    <mergeCell ref="Y171:AB171"/>
+    <mergeCell ref="AC171:AE171"/>
+    <mergeCell ref="AF171:AI171"/>
+    <mergeCell ref="AJ171:AL171"/>
+    <mergeCell ref="AM171:AP171"/>
+    <mergeCell ref="AQ171:AS171"/>
     <mergeCell ref="AT171:AW171"/>
     <mergeCell ref="AX171:AZ171"/>
     <mergeCell ref="BA171:BD171"/>
@@ -16007,75 +16087,6 @@
     <mergeCell ref="AQ170:AS170"/>
     <mergeCell ref="AQ6:AW6"/>
     <mergeCell ref="AX6:BD6"/>
-    <mergeCell ref="AL1:BD1"/>
-    <mergeCell ref="O1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="E171:G171"/>
-    <mergeCell ref="H171:J171"/>
-    <mergeCell ref="K171:N171"/>
-    <mergeCell ref="O171:Q171"/>
-    <mergeCell ref="R171:U171"/>
-    <mergeCell ref="V171:X171"/>
-    <mergeCell ref="Y171:AB171"/>
-    <mergeCell ref="AC171:AE171"/>
-    <mergeCell ref="AF171:AI171"/>
-    <mergeCell ref="AJ171:AL171"/>
-    <mergeCell ref="AM171:AP171"/>
-    <mergeCell ref="AQ171:AS171"/>
-    <mergeCell ref="E172:G172"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:Q3"/>
-    <mergeCell ref="I4:Q4"/>
-    <mergeCell ref="H172:J172"/>
-    <mergeCell ref="K172:N172"/>
-    <mergeCell ref="O172:Q172"/>
-    <mergeCell ref="H170:J170"/>
-    <mergeCell ref="K170:N170"/>
-    <mergeCell ref="O170:Q170"/>
-    <mergeCell ref="AQ172:AS172"/>
-    <mergeCell ref="AT172:AW172"/>
-    <mergeCell ref="AX172:AZ172"/>
-    <mergeCell ref="BA172:BD172"/>
-    <mergeCell ref="Y172:AB172"/>
-    <mergeCell ref="AC172:AE172"/>
-    <mergeCell ref="AF172:AI172"/>
-    <mergeCell ref="AJ172:AL172"/>
-    <mergeCell ref="AM172:AP172"/>
-    <mergeCell ref="R172:U172"/>
-    <mergeCell ref="V172:X172"/>
-    <mergeCell ref="Y170:AB170"/>
-    <mergeCell ref="AC170:AE170"/>
-    <mergeCell ref="AF170:AI170"/>
-    <mergeCell ref="V170:X170"/>
-    <mergeCell ref="R170:U170"/>
-    <mergeCell ref="A104:A168"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A87:A102"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A37:A74"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="AJ6:AP6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A15:A30"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="V6:AB6"/>
-    <mergeCell ref="AC6:AI6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -16095,10 +16106,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BX44"/>
+  <dimension ref="B1:BX43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="129" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="129" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16121,15 +16132,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="298" t="s">
+      <c r="C1" s="303" t="s">
         <v>351</v>
       </c>
-      <c r="D1" s="298"/>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
-      <c r="H1" s="298"/>
-      <c r="I1" s="298"/>
+      <c r="D1" s="303"/>
+      <c r="E1" s="303"/>
+      <c r="F1" s="303"/>
+      <c r="G1" s="303"/>
+      <c r="H1" s="303"/>
+      <c r="I1" s="303"/>
       <c r="J1" s="191"/>
       <c r="K1" s="211"/>
       <c r="L1" s="211"/>
@@ -16157,13 +16168,13 @@
     </row>
     <row r="2" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="191"/>
-      <c r="C2" s="298"/>
-      <c r="D2" s="298"/>
-      <c r="E2" s="298"/>
-      <c r="F2" s="298"/>
-      <c r="G2" s="298"/>
-      <c r="H2" s="298"/>
-      <c r="I2" s="298"/>
+      <c r="C2" s="303"/>
+      <c r="D2" s="303"/>
+      <c r="E2" s="303"/>
+      <c r="F2" s="303"/>
+      <c r="G2" s="303"/>
+      <c r="H2" s="303"/>
+      <c r="I2" s="303"/>
       <c r="J2" s="191"/>
       <c r="K2" s="211"/>
       <c r="L2" s="211"/>
@@ -16227,14 +16238,14 @@
       <c r="C4" s="200" t="s">
         <v>294</v>
       </c>
-      <c r="D4" s="296" t="s">
+      <c r="D4" s="301" t="s">
         <v>362</v>
       </c>
-      <c r="E4" s="296"/>
-      <c r="F4" s="296"/>
-      <c r="G4" s="296"/>
-      <c r="H4" s="296"/>
-      <c r="I4" s="297"/>
+      <c r="E4" s="301"/>
+      <c r="F4" s="301"/>
+      <c r="G4" s="301"/>
+      <c r="H4" s="301"/>
+      <c r="I4" s="302"/>
       <c r="J4" s="191"/>
       <c r="K4" s="211"/>
       <c r="L4" s="211"/>
@@ -16264,14 +16275,14 @@
       <c r="C5" s="200" t="s">
         <v>341</v>
       </c>
-      <c r="D5" s="296" t="s">
+      <c r="D5" s="301" t="s">
         <v>344</v>
       </c>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
-      <c r="G5" s="296"/>
-      <c r="H5" s="296"/>
-      <c r="I5" s="297"/>
+      <c r="E5" s="301"/>
+      <c r="F5" s="301"/>
+      <c r="G5" s="301"/>
+      <c r="H5" s="301"/>
+      <c r="I5" s="302"/>
       <c r="J5" s="191"/>
       <c r="K5" s="211"/>
       <c r="L5" s="211"/>
@@ -16299,12 +16310,12 @@
     </row>
     <row r="6" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="200"/>
-      <c r="D6" s="301"/>
-      <c r="E6" s="301"/>
-      <c r="F6" s="301"/>
-      <c r="G6" s="301"/>
-      <c r="H6" s="301"/>
-      <c r="I6" s="302"/>
+      <c r="D6" s="306"/>
+      <c r="E6" s="306"/>
+      <c r="F6" s="306"/>
+      <c r="G6" s="306"/>
+      <c r="H6" s="306"/>
+      <c r="I6" s="307"/>
       <c r="J6" s="191"/>
       <c r="K6" s="211"/>
       <c r="L6" s="211"/>
@@ -16335,14 +16346,14 @@
       <c r="C7" s="200" t="s">
         <v>357</v>
       </c>
-      <c r="D7" s="303" t="s">
+      <c r="D7" s="308" t="s">
         <v>350</v>
       </c>
-      <c r="E7" s="303"/>
-      <c r="F7" s="303"/>
-      <c r="G7" s="303"/>
-      <c r="H7" s="303"/>
-      <c r="I7" s="304"/>
+      <c r="E7" s="308"/>
+      <c r="F7" s="308"/>
+      <c r="G7" s="308"/>
+      <c r="H7" s="308"/>
+      <c r="I7" s="309"/>
       <c r="J7" s="191"/>
       <c r="K7" s="211"/>
       <c r="L7" s="211"/>
@@ -16407,12 +16418,12 @@
       <c r="C9" s="198" t="s">
         <v>363</v>
       </c>
-      <c r="D9" s="296"/>
-      <c r="E9" s="296"/>
-      <c r="F9" s="296"/>
-      <c r="G9" s="296"/>
-      <c r="H9" s="296"/>
-      <c r="I9" s="297"/>
+      <c r="D9" s="301"/>
+      <c r="E9" s="301"/>
+      <c r="F9" s="301"/>
+      <c r="G9" s="301"/>
+      <c r="H9" s="301"/>
+      <c r="I9" s="302"/>
       <c r="J9" s="191"/>
       <c r="K9" s="211"/>
       <c r="L9" s="211"/>
@@ -16477,12 +16488,12 @@
         <v>352</v>
       </c>
       <c r="D11" s="226"/>
-      <c r="F11" s="307" t="s">
+      <c r="F11" s="312" t="s">
         <v>355</v>
       </c>
-      <c r="G11" s="308"/>
-      <c r="H11" s="303"/>
-      <c r="I11" s="304"/>
+      <c r="G11" s="313"/>
+      <c r="H11" s="308"/>
+      <c r="I11" s="309"/>
       <c r="J11" s="191"/>
       <c r="K11" s="211"/>
       <c r="L11" s="211"/>
@@ -16513,12 +16524,12 @@
         <v>353</v>
       </c>
       <c r="D12" s="226"/>
-      <c r="F12" s="307" t="s">
+      <c r="F12" s="312" t="s">
         <v>356</v>
       </c>
-      <c r="G12" s="308"/>
-      <c r="H12" s="305"/>
-      <c r="I12" s="306"/>
+      <c r="G12" s="313"/>
+      <c r="H12" s="310"/>
+      <c r="I12" s="311"/>
       <c r="J12" s="191"/>
       <c r="K12" s="211"/>
       <c r="L12" s="211"/>
@@ -16608,14 +16619,14 @@
       <c r="C15" s="200" t="s">
         <v>358</v>
       </c>
-      <c r="D15" s="296" t="s">
+      <c r="D15" s="301" t="s">
         <v>360</v>
       </c>
-      <c r="E15" s="296"/>
-      <c r="F15" s="296"/>
-      <c r="G15" s="296"/>
-      <c r="H15" s="296"/>
-      <c r="I15" s="297"/>
+      <c r="E15" s="301"/>
+      <c r="F15" s="301"/>
+      <c r="G15" s="301"/>
+      <c r="H15" s="301"/>
+      <c r="I15" s="302"/>
       <c r="L15" s="211"/>
       <c r="M15" s="211"/>
       <c r="N15" s="211"/>
@@ -16639,14 +16650,14 @@
       <c r="C16" s="200" t="s">
         <v>359</v>
       </c>
-      <c r="D16" s="299" t="s">
+      <c r="D16" s="304" t="s">
         <v>361</v>
       </c>
-      <c r="E16" s="299"/>
-      <c r="F16" s="299"/>
-      <c r="G16" s="299"/>
-      <c r="H16" s="299"/>
-      <c r="I16" s="300"/>
+      <c r="E16" s="304"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="304"/>
+      <c r="H16" s="304"/>
+      <c r="I16" s="305"/>
       <c r="J16" s="191"/>
       <c r="K16" s="211"/>
       <c r="L16" s="211"/>
@@ -16696,15 +16707,15 @@
       <c r="AC17" s="211"/>
     </row>
     <row r="18" spans="2:33" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="284" t="s">
+      <c r="C18" s="314" t="s">
         <v>305</v>
       </c>
-      <c r="D18" s="285"/>
-      <c r="E18" s="285"/>
-      <c r="F18" s="285"/>
-      <c r="G18" s="285"/>
-      <c r="H18" s="286"/>
-      <c r="I18" s="287"/>
+      <c r="D18" s="315"/>
+      <c r="E18" s="315"/>
+      <c r="F18" s="315"/>
+      <c r="G18" s="315"/>
+      <c r="H18" s="316"/>
+      <c r="I18" s="317"/>
       <c r="K18" s="210"/>
       <c r="L18" s="210"/>
       <c r="M18" s="210"/>
@@ -16726,15 +16737,15 @@
       <c r="AC18" s="186"/>
     </row>
     <row r="19" spans="2:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="288" t="s">
+      <c r="C19" s="318" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="289"/>
-      <c r="E19" s="289"/>
-      <c r="F19" s="289"/>
-      <c r="G19" s="289"/>
-      <c r="H19" s="292"/>
-      <c r="I19" s="293"/>
+      <c r="D19" s="319"/>
+      <c r="E19" s="319"/>
+      <c r="F19" s="319"/>
+      <c r="G19" s="319"/>
+      <c r="H19" s="322"/>
+      <c r="I19" s="323"/>
       <c r="K19" s="210"/>
       <c r="L19" s="210"/>
       <c r="M19" s="210"/>
@@ -16756,18 +16767,18 @@
       <c r="AC19" s="186"/>
     </row>
     <row r="20" spans="2:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="290" t="s">
+      <c r="C20" s="320" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="291"/>
-      <c r="E20" s="291"/>
-      <c r="F20" s="291"/>
-      <c r="G20" s="291"/>
-      <c r="H20" s="294">
+      <c r="D20" s="321"/>
+      <c r="E20" s="321"/>
+      <c r="F20" s="321"/>
+      <c r="G20" s="321"/>
+      <c r="H20" s="324">
         <f>H18+H19</f>
         <v>0</v>
       </c>
-      <c r="I20" s="295"/>
+      <c r="I20" s="325"/>
       <c r="K20" s="210"/>
       <c r="L20" s="210"/>
       <c r="M20" s="210"/>
@@ -16811,22 +16822,22 @@
       <c r="AC21" s="186"/>
     </row>
     <row r="22" spans="2:33" s="182" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="309" t="s">
+      <c r="B22" s="281" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="319" t="s">
+      <c r="C22" s="291" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="321" t="s">
+      <c r="D22" s="293" t="s">
         <v>301</v>
       </c>
-      <c r="E22" s="322"/>
-      <c r="F22" s="322"/>
-      <c r="G22" s="322"/>
-      <c r="H22" s="322"/>
-      <c r="I22" s="323"/>
-      <c r="J22" s="317" t="s">
-        <v>368</v>
+      <c r="E22" s="294"/>
+      <c r="F22" s="294"/>
+      <c r="G22" s="294"/>
+      <c r="H22" s="294"/>
+      <c r="I22" s="295"/>
+      <c r="J22" s="289" t="s">
+        <v>367</v>
       </c>
       <c r="K22" s="239"/>
       <c r="L22" s="239"/>
@@ -16853,17 +16864,17 @@
       <c r="AG22" s="237"/>
     </row>
     <row r="23" spans="2:33" s="182" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="310"/>
-      <c r="C23" s="320"/>
-      <c r="D23" s="324" t="s">
+      <c r="B23" s="282"/>
+      <c r="C23" s="292"/>
+      <c r="D23" s="296" t="s">
         <v>340</v>
       </c>
-      <c r="E23" s="325"/>
-      <c r="F23" s="325"/>
-      <c r="G23" s="325"/>
-      <c r="H23" s="325"/>
-      <c r="I23" s="325"/>
-      <c r="J23" s="318"/>
+      <c r="E23" s="297"/>
+      <c r="F23" s="297"/>
+      <c r="G23" s="297"/>
+      <c r="H23" s="297"/>
+      <c r="I23" s="297"/>
+      <c r="J23" s="290"/>
       <c r="K23" s="236"/>
       <c r="L23" s="236"/>
       <c r="M23" s="236"/>
@@ -16889,49 +16900,49 @@
       <c r="AG23" s="237"/>
     </row>
     <row r="24" spans="2:33" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="310"/>
-      <c r="C24" s="320"/>
-      <c r="D24" s="313" t="s">
+      <c r="B24" s="282"/>
+      <c r="C24" s="292"/>
+      <c r="D24" s="285" t="s">
         <v>342</v>
       </c>
-      <c r="E24" s="313" t="s">
+      <c r="E24" s="285" t="s">
         <v>364</v>
       </c>
-      <c r="F24" s="281" t="s">
+      <c r="F24" s="298" t="s">
         <v>365</v>
       </c>
-      <c r="G24" s="281" t="s">
+      <c r="G24" s="298" t="s">
         <v>366</v>
       </c>
-      <c r="H24" s="281" t="s">
-        <v>367</v>
-      </c>
-      <c r="I24" s="313" t="s">
+      <c r="H24" s="298" t="s">
+        <v>369</v>
+      </c>
+      <c r="I24" s="285" t="s">
         <v>343</v>
       </c>
-      <c r="J24" s="318"/>
+      <c r="J24" s="290"/>
     </row>
     <row r="25" spans="2:33" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="310"/>
-      <c r="C25" s="320"/>
-      <c r="D25" s="313"/>
-      <c r="E25" s="313"/>
-      <c r="F25" s="282"/>
-      <c r="G25" s="282"/>
-      <c r="H25" s="282"/>
-      <c r="I25" s="313"/>
-      <c r="J25" s="318"/>
+      <c r="B25" s="282"/>
+      <c r="C25" s="292"/>
+      <c r="D25" s="285"/>
+      <c r="E25" s="285"/>
+      <c r="F25" s="299"/>
+      <c r="G25" s="299"/>
+      <c r="H25" s="299"/>
+      <c r="I25" s="285"/>
+      <c r="J25" s="290"/>
     </row>
     <row r="26" spans="2:33" s="182" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="311"/>
-      <c r="C26" s="320"/>
-      <c r="D26" s="314"/>
-      <c r="E26" s="314"/>
-      <c r="F26" s="283"/>
-      <c r="G26" s="283"/>
-      <c r="H26" s="283"/>
-      <c r="I26" s="314"/>
-      <c r="J26" s="318"/>
+      <c r="B26" s="283"/>
+      <c r="C26" s="292"/>
+      <c r="D26" s="286"/>
+      <c r="E26" s="286"/>
+      <c r="F26" s="300"/>
+      <c r="G26" s="300"/>
+      <c r="H26" s="300"/>
+      <c r="I26" s="286"/>
+      <c r="J26" s="290"/>
     </row>
     <row r="27" spans="2:33" s="182" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B27" s="212"/>
@@ -16978,9 +16989,9 @@
       <c r="I30" s="228">
         <v>23</v>
       </c>
-      <c r="J30" s="315"/>
-      <c r="K30" s="315"/>
-      <c r="L30" s="315"/>
+      <c r="J30" s="287"/>
+      <c r="K30" s="287"/>
+      <c r="L30" s="287"/>
       <c r="M30" s="210"/>
       <c r="N30" s="210"/>
       <c r="O30" s="210"/>
@@ -16990,13 +17001,13 @@
       <c r="S30" s="210"/>
       <c r="T30" s="210"/>
       <c r="U30" s="210"/>
-      <c r="V30" s="312"/>
-      <c r="W30" s="312"/>
-      <c r="X30" s="316"/>
-      <c r="Y30" s="316"/>
-      <c r="Z30" s="316"/>
-      <c r="AA30" s="316"/>
-      <c r="AB30" s="316"/>
+      <c r="V30" s="284"/>
+      <c r="W30" s="284"/>
+      <c r="X30" s="288"/>
+      <c r="Y30" s="288"/>
+      <c r="Z30" s="288"/>
+      <c r="AA30" s="288"/>
+      <c r="AB30" s="288"/>
       <c r="AC30" s="210"/>
     </row>
     <row r="31" spans="2:33" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17042,9 +17053,9 @@
       <c r="I32" s="234">
         <v>123</v>
       </c>
-      <c r="J32" s="315"/>
-      <c r="K32" s="315"/>
-      <c r="L32" s="315"/>
+      <c r="J32" s="287"/>
+      <c r="K32" s="287"/>
+      <c r="L32" s="287"/>
       <c r="M32" s="210"/>
       <c r="N32" s="210"/>
       <c r="O32" s="210"/>
@@ -17055,9 +17066,9 @@
       <c r="T32" s="210"/>
       <c r="U32" s="210"/>
       <c r="V32" s="210"/>
-      <c r="W32" s="316"/>
-      <c r="X32" s="316"/>
-      <c r="Y32" s="316"/>
+      <c r="W32" s="288"/>
+      <c r="X32" s="288"/>
+      <c r="Y32" s="288"/>
       <c r="Z32" s="210"/>
       <c r="AA32" s="210"/>
       <c r="AB32" s="210"/>
@@ -17066,14 +17077,16 @@
     <row r="33" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="181"/>
       <c r="C33" s="205" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D33" s="206"/>
       <c r="E33" s="206"/>
       <c r="F33" s="206"/>
       <c r="G33" s="206"/>
       <c r="H33" s="229"/>
-      <c r="I33" s="234"/>
+      <c r="I33" s="234">
+        <v>123</v>
+      </c>
       <c r="J33" s="209"/>
       <c r="K33" s="209"/>
       <c r="L33" s="209"/>
@@ -17097,13 +17110,17 @@
     </row>
     <row r="34" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="181"/>
-      <c r="C34" s="205"/>
-      <c r="D34" s="206"/>
-      <c r="E34" s="206"/>
-      <c r="F34" s="206"/>
-      <c r="G34" s="206"/>
+      <c r="C34" s="203" t="s">
+        <v>347</v>
+      </c>
+      <c r="D34" s="204"/>
+      <c r="E34" s="204"/>
+      <c r="F34" s="204"/>
+      <c r="G34" s="204"/>
       <c r="H34" s="229"/>
-      <c r="I34" s="228"/>
+      <c r="I34" s="233">
+        <v>123</v>
+      </c>
       <c r="J34" s="210"/>
       <c r="K34" s="210"/>
       <c r="L34" s="210"/>
@@ -17117,73 +17134,57 @@
       <c r="T34" s="210"/>
       <c r="U34" s="210"/>
       <c r="V34" s="210"/>
-      <c r="W34" s="312"/>
-      <c r="X34" s="312"/>
-      <c r="Y34" s="312"/>
-      <c r="Z34" s="312"/>
-      <c r="AA34" s="312"/>
+      <c r="W34" s="210"/>
+      <c r="X34" s="210"/>
+      <c r="Y34" s="210"/>
+      <c r="Z34" s="210"/>
+      <c r="AA34" s="210"/>
       <c r="AB34" s="210"/>
       <c r="AC34" s="210"/>
     </row>
     <row r="35" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="181"/>
-      <c r="C35" s="203" t="s">
-        <v>347</v>
-      </c>
-      <c r="D35" s="204"/>
-      <c r="E35" s="204"/>
-      <c r="F35" s="204"/>
-      <c r="G35" s="204"/>
+      <c r="C35" s="207" t="s">
+        <v>349</v>
+      </c>
+      <c r="D35" s="208"/>
+      <c r="E35" s="208"/>
+      <c r="F35" s="208"/>
+      <c r="G35" s="208"/>
       <c r="H35" s="229"/>
-      <c r="I35" s="233">
+      <c r="I35" s="235">
         <v>123</v>
       </c>
-      <c r="J35" s="210"/>
-      <c r="K35" s="210"/>
-      <c r="L35" s="210"/>
-      <c r="M35" s="210"/>
-      <c r="N35" s="210"/>
-      <c r="O35" s="210"/>
-      <c r="P35" s="210"/>
-      <c r="Q35" s="210"/>
-      <c r="R35" s="210"/>
-      <c r="S35" s="210"/>
-      <c r="T35" s="210"/>
-      <c r="U35" s="210"/>
-      <c r="V35" s="210"/>
-      <c r="W35" s="210"/>
-      <c r="X35" s="210"/>
-      <c r="Y35" s="210"/>
-      <c r="Z35" s="210"/>
-      <c r="AA35" s="210"/>
-      <c r="AB35" s="210"/>
-      <c r="AC35" s="210"/>
-    </row>
-    <row r="36" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="207" t="s">
-        <v>349</v>
-      </c>
-      <c r="D36" s="208"/>
-      <c r="E36" s="208"/>
-      <c r="F36" s="208"/>
-      <c r="G36" s="208"/>
-      <c r="H36" s="229"/>
-      <c r="I36" s="235">
-        <v>123</v>
-      </c>
-      <c r="J36" s="184"/>
-      <c r="W36" s="240"/>
+      <c r="J35" s="184"/>
+      <c r="W35" s="240"/>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C42" s="185"/>
     </row>
     <row r="43" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C43" s="185"/>
     </row>
-    <row r="44" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C44" s="185"/>
-    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="34">
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="C1:I2"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D16:I16"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="B22:B26"/>
-    <mergeCell ref="W34:AA34"/>
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J32:L32"/>
@@ -17198,25 +17199,6 @@
     <mergeCell ref="D23:I23"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="G24:G26"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="C1:I2"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="D16:I16"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="P30">

</xml_diff>